<commit_message>
append Decision Tree, ANN and ANN Ensemble for Pattern 1 and Pattern 2
</commit_message>
<xml_diff>
--- a/processing_directory/results/prediction_result.xlsx
+++ b/processing_directory/results/prediction_result.xlsx
@@ -716,10 +716,10 @@
         <v>0.2272470198638459</v>
       </c>
       <c r="S4" t="n">
-        <v>0.2073297006341418</v>
+        <v>0.2073297006341419</v>
       </c>
       <c r="T4" t="n">
-        <v>0.2053152332281133</v>
+        <v>0.2053152332281132</v>
       </c>
     </row>
     <row r="5">
@@ -902,7 +902,7 @@
         <v>0.1931893647496956</v>
       </c>
       <c r="S7" t="n">
-        <v>0.2231156235527192</v>
+        <v>0.2231156235527191</v>
       </c>
       <c r="T7" t="n">
         <v>0.2377869295562779</v>
@@ -964,10 +964,10 @@
         <v>0.2346849395877877</v>
       </c>
       <c r="S8" t="n">
-        <v>0.2219067922035781</v>
+        <v>0.221906792203578</v>
       </c>
       <c r="T8" t="n">
-        <v>0.2254189992112531</v>
+        <v>0.225418999211253</v>
       </c>
     </row>
     <row r="9">
@@ -1212,10 +1212,10 @@
         <v>0.2157948102296876</v>
       </c>
       <c r="S12" t="n">
-        <v>0.2314083933858393</v>
+        <v>0.2314083933858394</v>
       </c>
       <c r="T12" t="n">
-        <v>0.2307123677801181</v>
+        <v>0.230712367780118</v>
       </c>
     </row>
     <row r="13">
@@ -1277,7 +1277,7 @@
         <v>0.200904665905617</v>
       </c>
       <c r="T13" t="n">
-        <v>0.2065069651315891</v>
+        <v>0.206506965131589</v>
       </c>
     </row>
     <row r="14">
@@ -1463,7 +1463,7 @@
         <v>0.2180481254158904</v>
       </c>
       <c r="T16" t="n">
-        <v>0.2338077038630101</v>
+        <v>0.23380770386301</v>
       </c>
     </row>
     <row r="17">
@@ -1522,7 +1522,7 @@
         <v>0.1996672995189508</v>
       </c>
       <c r="S17" t="n">
-        <v>0.2055767598256379</v>
+        <v>0.2055767598256378</v>
       </c>
       <c r="T17" t="n">
         <v>0.2093021527103635</v>
@@ -1897,7 +1897,7 @@
         <v>0.2733873727770533</v>
       </c>
       <c r="T23" t="n">
-        <v>0.2792220035167618</v>
+        <v>0.2792220035167617</v>
       </c>
     </row>
     <row r="24">
@@ -2207,7 +2207,7 @@
         <v>0.2337944102405378</v>
       </c>
       <c r="T28" t="n">
-        <v>0.2408295181036397</v>
+        <v>0.2408295181036398</v>
       </c>
     </row>
     <row r="29">
@@ -2393,7 +2393,7 @@
         <v>0.2226573148273891</v>
       </c>
       <c r="T31" t="n">
-        <v>0.2251216554156628</v>
+        <v>0.2251216554156627</v>
       </c>
     </row>
     <row r="32">
@@ -2703,7 +2703,7 @@
         <v>0.2190980751151007</v>
       </c>
       <c r="T36" t="n">
-        <v>0.2181892769391572</v>
+        <v>0.2181892769391571</v>
       </c>
     </row>
     <row r="37">
@@ -2762,7 +2762,7 @@
         <v>0.2586208678631206</v>
       </c>
       <c r="S37" t="n">
-        <v>0.2687632841050188</v>
+        <v>0.2687632841050187</v>
       </c>
       <c r="T37" t="n">
         <v>0.253277106117451</v>
@@ -2889,7 +2889,7 @@
         <v>0.2340887382513701</v>
       </c>
       <c r="T39" t="n">
-        <v>0.2262037098469677</v>
+        <v>0.2262037098469676</v>
       </c>
     </row>
     <row r="40">
@@ -3075,7 +3075,7 @@
         <v>0.2013160987103029</v>
       </c>
       <c r="T42" t="n">
-        <v>0.2099764893759976</v>
+        <v>0.2099764893759975</v>
       </c>
     </row>
     <row r="43">
@@ -3382,10 +3382,10 @@
         <v>0.1791811870722695</v>
       </c>
       <c r="S47" t="n">
-        <v>0.1620788740165244</v>
+        <v>0.1620788740165243</v>
       </c>
       <c r="T47" t="n">
-        <v>0.1164067509224005</v>
+        <v>0.1164067509224004</v>
       </c>
     </row>
     <row r="48">
@@ -3754,10 +3754,10 @@
         <v>0.1391748365370473</v>
       </c>
       <c r="S53" t="n">
-        <v>0.1505660588878692</v>
+        <v>0.1505660588878691</v>
       </c>
       <c r="T53" t="n">
-        <v>0.1416905309138031</v>
+        <v>0.1416905309138032</v>
       </c>
     </row>
     <row r="54">
@@ -4126,7 +4126,7 @@
         <v>0.1865291868067152</v>
       </c>
       <c r="S59" t="n">
-        <v>0.1861627874706829</v>
+        <v>0.1861627874706828</v>
       </c>
       <c r="T59" t="n">
         <v>0.1745830975305752</v>
@@ -4374,10 +4374,10 @@
         <v>0.1786848223279511</v>
       </c>
       <c r="S63" t="n">
-        <v>0.1678390723043481</v>
+        <v>0.1678390723043482</v>
       </c>
       <c r="T63" t="n">
-        <v>0.1587309088407478</v>
+        <v>0.1587309088407477</v>
       </c>
     </row>
     <row r="64">
@@ -4498,7 +4498,7 @@
         <v>0.1472035166429491</v>
       </c>
       <c r="S65" t="n">
-        <v>0.1701901082445679</v>
+        <v>0.170190108244568</v>
       </c>
       <c r="T65" t="n">
         <v>0.1730015378768515</v>
@@ -4932,7 +4932,7 @@
         <v>0.1666777951542437</v>
       </c>
       <c r="S72" t="n">
-        <v>0.1811532958346611</v>
+        <v>0.1811532958346612</v>
       </c>
       <c r="T72" t="n">
         <v>0.188424045872836</v>
@@ -5121,7 +5121,7 @@
         <v>0.1760161577558566</v>
       </c>
       <c r="T75" t="n">
-        <v>0.1812588184477431</v>
+        <v>0.181258818447743</v>
       </c>
     </row>
     <row r="76">
@@ -5431,7 +5431,7 @@
         <v>0.1386020125929636</v>
       </c>
       <c r="T80" t="n">
-        <v>0.1320982015023293</v>
+        <v>0.1320982015023292</v>
       </c>
     </row>
     <row r="81">
@@ -5490,7 +5490,7 @@
         <v>0.1753952188044234</v>
       </c>
       <c r="S81" t="n">
-        <v>0.196068878860898</v>
+        <v>0.1960688788608979</v>
       </c>
       <c r="T81" t="n">
         <v>0.1993644097300707</v>
@@ -5555,7 +5555,7 @@
         <v>0.2214128534186159</v>
       </c>
       <c r="T82" t="n">
-        <v>0.2248935544199317</v>
+        <v>0.2248935544199316</v>
       </c>
     </row>
     <row r="83">
@@ -6048,7 +6048,7 @@
         <v>0.2252853065527711</v>
       </c>
       <c r="S90" t="n">
-        <v>0.2160070173606579</v>
+        <v>0.2160070173606578</v>
       </c>
       <c r="T90" t="n">
         <v>0.2231820668898817</v>
@@ -6234,7 +6234,7 @@
         <v>0.2216153961929441</v>
       </c>
       <c r="S93" t="n">
-        <v>0.2204289744470796</v>
+        <v>0.2204289744470797</v>
       </c>
       <c r="T93" t="n">
         <v>0.2208268685526975</v>
@@ -6296,10 +6296,10 @@
         <v>0.3109674760178356</v>
       </c>
       <c r="S94" t="n">
-        <v>0.2735429570770335</v>
+        <v>0.2735429570770334</v>
       </c>
       <c r="T94" t="n">
-        <v>0.2659089435180005</v>
+        <v>0.2659089435180004</v>
       </c>
     </row>
     <row r="95">
@@ -6358,10 +6358,10 @@
         <v>0.2645657224059876</v>
       </c>
       <c r="S95" t="n">
-        <v>0.2550232515092382</v>
+        <v>0.2550232515092383</v>
       </c>
       <c r="T95" t="n">
-        <v>0.2625783842369382</v>
+        <v>0.2625783842369383</v>
       </c>
     </row>
     <row r="96">
@@ -6420,7 +6420,7 @@
         <v>0.268506805750846</v>
       </c>
       <c r="S96" t="n">
-        <v>0.253459316908745</v>
+        <v>0.2534593169087449</v>
       </c>
       <c r="T96" t="n">
         <v>0.2661438238221684</v>
@@ -6730,7 +6730,7 @@
         <v>0.2143726836255242</v>
       </c>
       <c r="S101" t="n">
-        <v>0.2665992680988932</v>
+        <v>0.2665992680988933</v>
       </c>
       <c r="T101" t="n">
         <v>0.2705624972194197</v>
@@ -6792,10 +6792,10 @@
         <v>0.1987337698920451</v>
       </c>
       <c r="S102" t="n">
-        <v>0.2635436264339372</v>
+        <v>0.2635436264339371</v>
       </c>
       <c r="T102" t="n">
-        <v>0.2643671933654005</v>
+        <v>0.2643671933654004</v>
       </c>
     </row>
     <row r="103">
@@ -6857,7 +6857,7 @@
         <v>0.1873886993048487</v>
       </c>
       <c r="T103" t="n">
-        <v>0.1924671103896302</v>
+        <v>0.1924671103896303</v>
       </c>
     </row>
     <row r="104">
@@ -6919,7 +6919,7 @@
         <v>0.1586004926555664</v>
       </c>
       <c r="T104" t="n">
-        <v>0.1811603168898202</v>
+        <v>0.1811603168898201</v>
       </c>
     </row>
     <row r="105">
@@ -7043,7 +7043,7 @@
         <v>0.1354644136561511</v>
       </c>
       <c r="T106" t="n">
-        <v>0.1352302077784681</v>
+        <v>0.135230207778468</v>
       </c>
     </row>
     <row r="107">
@@ -7226,7 +7226,7 @@
         <v>0.1750233653857247</v>
       </c>
       <c r="S109" t="n">
-        <v>0.1678765449998169</v>
+        <v>0.167876544999817</v>
       </c>
       <c r="T109" t="n">
         <v>0.1727932240839123</v>
@@ -7350,7 +7350,7 @@
         <v>0.2036316124785982</v>
       </c>
       <c r="S111" t="n">
-        <v>0.1897779066676337</v>
+        <v>0.1897779066676336</v>
       </c>
       <c r="T111" t="n">
         <v>0.1876968090977955</v>
@@ -7601,7 +7601,7 @@
         <v>0.1626368831227729</v>
       </c>
       <c r="T115" t="n">
-        <v>0.1694376779875491</v>
+        <v>0.1694376779875492</v>
       </c>
     </row>
     <row r="116">
@@ -7660,7 +7660,7 @@
         <v>0.1439429260567104</v>
       </c>
       <c r="S116" t="n">
-        <v>0.1535053081107759</v>
+        <v>0.153505308110776</v>
       </c>
       <c r="T116" t="n">
         <v>0.1211292508039283</v>
@@ -7908,7 +7908,7 @@
         <v>0.1461658668775163</v>
       </c>
       <c r="S120" t="n">
-        <v>0.1646322324531717</v>
+        <v>0.1646322324531716</v>
       </c>
       <c r="T120" t="n">
         <v>0.1690189876253287</v>
@@ -8032,7 +8032,7 @@
         <v>0.1796703213986381</v>
       </c>
       <c r="S122" t="n">
-        <v>0.1487621311827615</v>
+        <v>0.1487621311827614</v>
       </c>
       <c r="T122" t="n">
         <v>0.1372327375114101</v>

</xml_diff>